<commit_message>
Final Commit before changing to new metabolomics data
</commit_message>
<xml_diff>
--- a/Supporting files/superpathway_key.xlsx
+++ b/Supporting files/superpathway_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagoodri\Desktop\MetaAir_AP\Supporting files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagoodri\Dropbox (USC Lab)\Project Directories\SOLAR CHS Metabolomics Analysis\1_Code\Supporting files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191F9227-DD2E-471F-9924-153AFC607120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC57EBD-9348-43AC-87C7-A4E68F0824EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="29760" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="29988" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="superpathway_key" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
   <si>
     <t>super_pathway</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>3-oxo-10R-octadecatrienoate beta-oxidation</t>
+  </si>
+  <si>
+    <t>Glycolysis and Gluconeogenesis</t>
   </si>
 </sst>
 </file>
@@ -1112,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,6 +1718,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>